<commit_message>
add view table laporan lipa 5
</commit_message>
<xml_diff>
--- a/hasil/2023_01_lipa_5.xlsx
+++ b/hasil/2023_01_lipa_5.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="53">
   <si>
     <t>LAPORAN PERKARA YANG DIMOHONKAN EKSEKUSI</t>
   </si>
@@ -100,21 +100,6 @@
     <t>14</t>
   </si>
   <si>
-    <t>3/Pdt.Eks/2020/PA.Tte</t>
-  </si>
-  <si>
-    <t>2/Pdt.G/2019/PTA.MU</t>
-  </si>
-  <si>
-    <t>04/11/2020</t>
-  </si>
-  <si>
-    <t>18/11/2020</t>
-  </si>
-  <si>
-    <t>25/11/2020</t>
-  </si>
-  <si>
     <t>2/Pdt.Eks/2022/PA.Tte</t>
   </si>
   <si>
@@ -154,6 +139,9 @@
     <t>28/06/2021</t>
   </si>
   <si>
+    <t>11/01/2023</t>
+  </si>
+  <si>
     <t>3/Pdt.Eks/2022/PA.Tte</t>
   </si>
   <si>
@@ -169,7 +157,7 @@
     <t>Mengetahui</t>
   </si>
   <si>
-    <t>Ternate , 02 Agustus 2023</t>
+    <t>Ternate , 04 September 2023</t>
   </si>
   <si>
     <t>Ketua Pengadilan Agama Ternate ,</t>
@@ -745,10 +733,10 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:N23"/>
+  <dimension ref="A1:N22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" view="pageBreakPreview" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr customHeight="true" defaultRowHeight="12.75" defaultColWidth="8.85546875" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -977,9 +965,15 @@
       <c r="F10" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="G10" s="17"/>
-      <c r="H10" s="17"/>
-      <c r="I10" s="17"/>
+      <c r="G10" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="H10" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="I10" s="17" t="s">
+        <v>34</v>
+      </c>
       <c r="J10" s="17"/>
       <c r="K10" s="17"/>
       <c r="L10" s="17"/>
@@ -991,30 +985,26 @@
         <v>2</v>
       </c>
       <c r="B11" s="17" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="C11" s="17" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="D11" s="17" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="E11" s="17" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="F11" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="G11" s="17" t="s">
-        <v>37</v>
-      </c>
-      <c r="H11" s="17" t="s">
-        <v>38</v>
-      </c>
-      <c r="I11" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="J11" s="17"/>
+      <c r="G11" s="17"/>
+      <c r="H11" s="17"/>
+      <c r="I11" s="17"/>
+      <c r="J11" s="17" t="s">
+        <v>40</v>
+      </c>
       <c r="K11" s="17"/>
       <c r="L11" s="17"/>
       <c r="M11" s="17"/>
@@ -1025,11 +1015,9 @@
         <v>3</v>
       </c>
       <c r="B12" s="17" t="s">
-        <v>40</v>
-      </c>
-      <c r="C12" s="17" t="s">
         <v>41</v>
       </c>
+      <c r="C12" s="17"/>
       <c r="D12" s="17" t="s">
         <v>42</v>
       </c>
@@ -1048,35 +1036,23 @@
       <c r="M12" s="17"/>
       <c r="N12" s="17"/>
     </row>
-    <row r="13" spans="1:14" customHeight="1" ht="25">
-      <c r="A13" s="17">
-        <v>4</v>
-      </c>
-      <c r="B13" s="17" t="s">
+    <row r="15" spans="1:14" customHeight="1" ht="20">
+      <c r="C15" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="C13" s="17"/>
-      <c r="D13" s="17" t="s">
+      <c r="D15" s="18"/>
+      <c r="E15" s="18"/>
+      <c r="F15" s="18"/>
+      <c r="G15" s="18"/>
+      <c r="H15" s="18"/>
+      <c r="I15" s="18"/>
+      <c r="J15" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="E13" s="17" t="s">
-        <v>47</v>
-      </c>
-      <c r="F13" s="17" t="s">
-        <v>48</v>
-      </c>
-      <c r="G13" s="17"/>
-      <c r="H13" s="17"/>
-      <c r="I13" s="17"/>
-      <c r="J13" s="17"/>
-      <c r="K13" s="17"/>
-      <c r="L13" s="17"/>
-      <c r="M13" s="17"/>
-      <c r="N13" s="17"/>
     </row>
     <row r="16" spans="1:14" customHeight="1" ht="20">
       <c r="C16" s="18" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D16" s="18"/>
       <c r="E16" s="18"/>
@@ -1085,22 +1061,18 @@
       <c r="H16" s="18"/>
       <c r="I16" s="18"/>
       <c r="J16" s="18" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="17" spans="1:14" customHeight="1" ht="20">
-      <c r="C17" s="18" t="s">
-        <v>51</v>
-      </c>
+        <v>48</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14">
+      <c r="C17" s="18"/>
       <c r="D17" s="18"/>
       <c r="E17" s="18"/>
       <c r="F17" s="18"/>
       <c r="G17" s="18"/>
       <c r="H17" s="18"/>
       <c r="I17" s="18"/>
-      <c r="J17" s="18" t="s">
-        <v>52</v>
-      </c>
+      <c r="J17" s="18"/>
     </row>
     <row r="18" spans="1:14">
       <c r="C18" s="18"/>
@@ -1132,19 +1104,23 @@
       <c r="I20" s="18"/>
       <c r="J20" s="18"/>
     </row>
-    <row r="21" spans="1:14">
-      <c r="C21" s="18"/>
+    <row r="21" spans="1:14" customHeight="1" ht="20">
+      <c r="C21" s="18" t="s">
+        <v>49</v>
+      </c>
       <c r="D21" s="18"/>
       <c r="E21" s="18"/>
       <c r="F21" s="18"/>
       <c r="G21" s="18"/>
       <c r="H21" s="18"/>
       <c r="I21" s="18"/>
-      <c r="J21" s="18"/>
+      <c r="J21" s="18" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="22" spans="1:14" customHeight="1" ht="20">
       <c r="C22" s="18" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D22" s="18"/>
       <c r="E22" s="18"/>
@@ -1153,21 +1129,7 @@
       <c r="H22" s="18"/>
       <c r="I22" s="18"/>
       <c r="J22" s="18" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="23" spans="1:14" customHeight="1" ht="20">
-      <c r="C23" s="18" t="s">
-        <v>55</v>
-      </c>
-      <c r="D23" s="18"/>
-      <c r="E23" s="18"/>
-      <c r="F23" s="18"/>
-      <c r="G23" s="18"/>
-      <c r="H23" s="18"/>
-      <c r="I23" s="18"/>
-      <c r="J23" s="18" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>